<commit_message>
Added ml model for variable importance
</commit_message>
<xml_diff>
--- a/data/atr_raw/ATR_2009-2021_clean.xlsx
+++ b/data/atr_raw/ATR_2009-2021_clean.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26505"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0"/>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{7D1CB1AF-FB74-469F-AFCA-79E49A8AC2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAE38854-A196-4F00-A4DD-0D6B19FAFCDE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0118AF-60C2-4D08-8DCF-7FF6CE263CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="524" yWindow="5068" windowWidth="26930" windowHeight="14325" tabRatio="678" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="678" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ATR-I.1.3" sheetId="5" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>total</t>
   </si>
   <si>
-    <t>agrario</t>
-  </si>
-  <si>
     <t>industria</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>region</t>
+  </si>
+  <si>
+    <t>agricultura</t>
   </si>
 </sst>
 </file>
@@ -422,10 +422,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -692,18 +688,18 @@
   <dimension ref="A1:O106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <pane ySplit="7" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27:A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="12.65" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="32.1640625" style="1" customWidth="1"/>
-    <col min="3" max="13" width="7.83203125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.5" style="1"/>
+    <col min="1" max="2" width="32.1328125" style="1" customWidth="1"/>
+    <col min="3" max="13" width="7.796875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.46484375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -718,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="5.3" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="5.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="5"/>
@@ -733,7 +729,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -750,7 +746,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
@@ -767,7 +763,7 @@
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -782,7 +778,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
@@ -799,12 +795,12 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="C7" s="19">
         <v>2009</v>
@@ -846,7 +842,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>23</v>
       </c>
@@ -893,7 +889,7 @@
         <v>2810.4882237364322</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>23</v>
       </c>
@@ -940,7 +936,7 @@
         <v>2949.6924171259543</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
@@ -987,7 +983,7 @@
         <v>2919.490743087279</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
@@ -1034,7 +1030,7 @@
         <v>2880.6006985750973</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>23</v>
       </c>
@@ -1081,7 +1077,7 @@
         <v>3785.5569746826409</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1128,7 +1124,7 @@
         <v>2354.3247684613034</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>23</v>
       </c>
@@ -1175,7 +1171,7 @@
         <v>2815.3853876875337</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>23</v>
       </c>
@@ -1222,7 +1218,7 @@
         <v>3726.2362985606874</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>23</v>
       </c>
@@ -1269,7 +1265,7 @@
         <v>2828.1212087767967</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>23</v>
       </c>
@@ -1316,7 +1312,7 @@
         <v>2670.6516471089308</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>23</v>
       </c>
@@ -1363,7 +1359,7 @@
         <v>2784.8157939961466</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>23</v>
       </c>
@@ -1410,7 +1406,7 @@
         <v>2978.9930724169535</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>23</v>
       </c>
@@ -1457,7 +1453,7 @@
         <v>2922.2943572030845</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
         <v>23</v>
       </c>
@@ -1504,7 +1500,7 @@
         <v>2228.974015866479</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>23</v>
       </c>
@@ -1551,7 +1547,7 @@
         <v>3199.6733651867462</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
         <v>23</v>
       </c>
@@ -1598,7 +1594,7 @@
         <v>3685.5136155250548</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
         <v>23</v>
       </c>
@@ -1645,7 +1641,7 @@
         <v>3196.4532810423111</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
         <v>23</v>
       </c>
@@ -1692,7 +1688,7 @@
         <v>3637.4544843532499</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>23</v>
       </c>
@@ -1739,9 +1735,9 @@
         <v>2708.9259108763376</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>23</v>
@@ -1786,9 +1782,9 @@
         <v>4318.6959855466012</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>3</v>
@@ -1833,9 +1829,9 @@
         <v>3994.4079866380662</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>4</v>
@@ -1880,9 +1876,9 @@
         <v>4058.7856250048521</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>5</v>
@@ -1927,9 +1923,9 @@
         <v>4713.6166417661734</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>6</v>
@@ -1974,9 +1970,9 @@
         <v>4778.7926347676803</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>7</v>
@@ -2021,9 +2017,9 @@
         <v>5426.2911651540135</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>8</v>
@@ -2068,9 +2064,9 @@
         <v>5029.592046333677</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>9</v>
@@ -2115,9 +2111,9 @@
         <v>4163.4650203580541</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>10</v>
@@ -2162,9 +2158,9 @@
         <v>3390.5160964904589</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>11</v>
@@ -2209,9 +2205,9 @@
         <v>3826.2885430134688</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>12</v>
@@ -2256,9 +2252,9 @@
         <v>5432.751469850964</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>13</v>
@@ -2303,9 +2299,9 @@
         <v>5353.1031769450183</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>14</v>
@@ -2350,9 +2346,9 @@
         <v>4246.6506051671731</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>15</v>
@@ -2397,9 +2393,9 @@
         <v>3870.203422027957</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>16</v>
@@ -2444,9 +2440,9 @@
         <v>4695.2939654568781</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>17</v>
@@ -2491,9 +2487,9 @@
         <v>4793.673147076257</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>18</v>
@@ -2538,9 +2534,9 @@
         <v>5667.3338696428309</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B44" s="16" t="s">
         <v>19</v>
@@ -2585,9 +2581,9 @@
         <v>4135.4426866500135</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>20</v>
@@ -2632,9 +2628,9 @@
         <v>6504.0650406504064</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>23</v>
@@ -2679,9 +2675,9 @@
         <v>4426.0184433656405</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>3</v>
@@ -2726,9 +2722,9 @@
         <v>4719.6996807075384</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" s="16" t="s">
         <v>4</v>
@@ -2773,9 +2769,9 @@
         <v>4077.7280734250958</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>5</v>
@@ -2820,9 +2816,9 @@
         <v>4703.960275629126</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>6</v>
@@ -2867,9 +2863,9 @@
         <v>5999.2246489442878</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>7</v>
@@ -2914,9 +2910,9 @@
         <v>3709.5738967554325</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>8</v>
@@ -2961,9 +2957,9 @@
         <v>3493.7672540883982</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>9</v>
@@ -3008,9 +3004,9 @@
         <v>5284.2498292209139</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>10</v>
@@ -3055,9 +3051,9 @@
         <v>4425.8878580989203</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>11</v>
@@ -3102,9 +3098,9 @@
         <v>3933.0391389783467</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>12</v>
@@ -3149,9 +3145,9 @@
         <v>3726.1248506724605</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>13</v>
@@ -3196,9 +3192,9 @@
         <v>5141.004360635563</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>14</v>
@@ -3243,9 +3239,9 @@
         <v>5017.679490955371</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>15</v>
@@ -3290,9 +3286,9 @@
         <v>3697.415043637488</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>16</v>
@@ -3337,9 +3333,9 @@
         <v>5514.6930444140398</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>17</v>
@@ -3384,9 +3380,9 @@
         <v>5309.3056818700552</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B62" s="16" t="s">
         <v>18</v>
@@ -3431,9 +3427,9 @@
         <v>5471.9409712889501</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B63" s="16" t="s">
         <v>19</v>
@@ -3478,9 +3474,9 @@
         <v>4749.1150587284392</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B64" s="16" t="s">
         <v>20</v>
@@ -3525,9 +3521,9 @@
         <v>6332.4538258575194</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B65" s="18" t="s">
         <v>23</v>
@@ -3572,9 +3568,9 @@
         <v>6316.0381436151447</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>3</v>
@@ -3619,9 +3615,9 @@
         <v>7254.1020219767133</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>4</v>
@@ -3666,9 +3662,9 @@
         <v>5387.7835293705384</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B68" s="16" t="s">
         <v>5</v>
@@ -3713,9 +3709,9 @@
         <v>6273.4625953016757</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>6</v>
@@ -3760,9 +3756,9 @@
         <v>7841.0158846585828</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>7</v>
@@ -3807,9 +3803,9 @@
         <v>6275.0997024016788</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>8</v>
@@ -3854,9 +3850,9 @@
         <v>5717.8955453618692</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>9</v>
@@ -3901,9 +3897,9 @@
         <v>6755.3698822194647</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>10</v>
@@ -3948,9 +3944,9 @@
         <v>5718.4501138370533</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>11</v>
@@ -3995,9 +3991,9 @@
         <v>5873.8002269856152</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B75" s="16" t="s">
         <v>12</v>
@@ -4042,9 +4038,9 @@
         <v>6068.2301494593703</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B76" s="16" t="s">
         <v>13</v>
@@ -4089,9 +4085,9 @@
         <v>6424.1580190864443</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B77" s="16" t="s">
         <v>14</v>
@@ -4136,9 +4132,9 @@
         <v>6030.1893275952516</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B78" s="16" t="s">
         <v>15</v>
@@ -4183,9 +4179,9 @@
         <v>5973.6578505066373</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B79" s="16" t="s">
         <v>16</v>
@@ -4230,9 +4226,9 @@
         <v>6185.7785198198153</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B80" s="16" t="s">
         <v>17</v>
@@ -4277,9 +4273,9 @@
         <v>6400.1656647325844</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B81" s="16" t="s">
         <v>18</v>
@@ -4324,9 +4320,9 @@
         <v>6253.5898365891435</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B82" s="16" t="s">
         <v>19</v>
@@ -4371,9 +4367,9 @@
         <v>7050.060119065075</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B83" s="16" t="s">
         <v>20</v>
@@ -4418,9 +4414,9 @@
         <v>6033.9332040185318</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B84" s="18" t="s">
         <v>23</v>
@@ -4465,9 +4461,9 @@
         <v>2166.6669600926166</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B85" s="16" t="s">
         <v>3</v>
@@ -4512,9 +4508,9 @@
         <v>2217.041291951954</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B86" s="16" t="s">
         <v>4</v>
@@ -4559,9 +4555,9 @@
         <v>2291.9684446507076</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B87" s="16" t="s">
         <v>5</v>
@@ -4606,9 +4602,9 @@
         <v>2175.6339386896989</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B88" s="16" t="s">
         <v>6</v>
@@ -4653,9 +4649,9 @@
         <v>3026.0136889215287</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B89" s="16" t="s">
         <v>7</v>
@@ -4700,9 +4696,9 @@
         <v>1873.5454584083361</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B90" s="16" t="s">
         <v>8</v>
@@ -4747,9 +4743,9 @@
         <v>2319.0955279674313</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B91" s="16" t="s">
         <v>9</v>
@@ -4794,9 +4790,9 @@
         <v>2915.9132839145796</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B92" s="16" t="s">
         <v>10</v>
@@ -4841,9 +4837,9 @@
         <v>2140.8481656044355</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B93" s="16" t="s">
         <v>11</v>
@@ -4888,9 +4884,9 @@
         <v>2167.0720939769149</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B94" s="16" t="s">
         <v>12</v>
@@ -4935,9 +4931,9 @@
         <v>2181.9009338226929</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B95" s="16" t="s">
         <v>13</v>
@@ -4982,9 +4978,9 @@
         <v>1953.4705517527909</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B96" s="16" t="s">
         <v>14</v>
@@ -5029,9 +5025,9 @@
         <v>2079.2614865352421</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B97" s="16" t="s">
         <v>15</v>
@@ -5076,9 +5072,9 @@
         <v>1850.0546332912095</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B98" s="16" t="s">
         <v>16</v>
@@ -5123,9 +5119,9 @@
         <v>2206.3735162735161</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B99" s="16" t="s">
         <v>17</v>
@@ -5170,9 +5166,9 @@
         <v>2746.0964104912296</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B100" s="16" t="s">
         <v>18</v>
@@ -5217,9 +5213,9 @@
         <v>2340.4853192773617</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B101" s="16" t="s">
         <v>19</v>
@@ -5264,9 +5260,9 @@
         <v>2904.1058559025569</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B102" s="16" t="s">
         <v>20</v>
@@ -5311,22 +5307,22 @@
         <v>2258.3541880221487</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C104" s="9"/>
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>

</xml_diff>